<commit_message>
FIX: Ministerios con servicios, inlcuido Nivel Central
</commit_message>
<xml_diff>
--- a/applications/sectores_gubernamentales/Nomina Reparticiones Públicas.xlsx
+++ b/applications/sectores_gubernamentales/Nomina Reparticiones Públicas.xlsx
@@ -1,30 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rvalenzuela\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaime\Desktop\SUBDERE\Transferencia de Competencias\transferenciacompetencias\applications\sectores_gubernamentales\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1805CAF3-BFF4-4DC6-8418-4CF2106F3540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="179">
   <si>
     <t>Ministerio del Interior y Seguridad Pública</t>
   </si>
@@ -558,12 +570,15 @@
   </si>
   <si>
     <t>Servicio Nacional de Reinserción Social Juvenil</t>
+  </si>
+  <si>
+    <t>Nivel Central</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -890,19 +905,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="23" width="54.42578125" customWidth="1"/>
+    <col min="1" max="23" width="54.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -973,556 +988,627 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
+        <v>178</v>
+      </c>
+      <c r="F2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" t="s">
+        <v>178</v>
+      </c>
+      <c r="J2" t="s">
+        <v>178</v>
+      </c>
+      <c r="K2" t="s">
+        <v>178</v>
+      </c>
+      <c r="L2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M2" t="s">
+        <v>178</v>
+      </c>
+      <c r="N2" t="s">
+        <v>178</v>
+      </c>
+      <c r="O2" t="s">
+        <v>178</v>
+      </c>
+      <c r="P2" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>178</v>
+      </c>
+      <c r="R2" t="s">
+        <v>178</v>
+      </c>
+      <c r="S2" t="s">
+        <v>178</v>
+      </c>
+      <c r="T2" t="s">
+        <v>178</v>
+      </c>
+      <c r="U2" t="s">
+        <v>178</v>
+      </c>
+      <c r="V2" t="s">
+        <v>178</v>
+      </c>
+      <c r="W2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>142</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>153</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>125</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I3" t="s">
         <v>107</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J3" t="s">
         <v>99</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K3" t="s">
         <v>86</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L3" t="s">
         <v>45</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M3" t="s">
         <v>42</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N3" t="s">
         <v>38</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O3" t="s">
         <v>36</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P3" t="s">
         <v>26</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R3" t="s">
         <v>32</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S3" t="s">
         <v>30</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T3" t="s">
         <v>29</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U3" t="s">
         <v>28</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V3" t="s">
         <v>124</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>152</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>148</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>154</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>130</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G4" t="s">
         <v>126</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H4" t="s">
         <v>116</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I4" t="s">
         <v>108</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J4" t="s">
         <v>100</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K4" t="s">
         <v>87</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L4" t="s">
         <v>46</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M4" t="s">
         <v>163</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N4" t="s">
         <v>39</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O4" t="s">
         <v>37</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P4" t="s">
         <v>35</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R4" t="s">
         <v>33</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S4" t="s">
         <v>31</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U4" t="s">
         <v>150</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>151</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>149</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>155</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>131</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" t="s">
         <v>127</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H5" t="s">
         <v>117</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I5" t="s">
         <v>109</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J5" t="s">
         <v>101</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K5" t="s">
         <v>88</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L5" t="s">
         <v>47</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M5" t="s">
         <v>164</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N5" t="s">
         <v>40</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R5" t="s">
         <v>34</v>
       </c>
-      <c r="V4" t="s">
+      <c r="V5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>139</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>156</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>132</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>128</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H6" t="s">
         <v>118</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" t="s">
         <v>110</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J6" t="s">
         <v>102</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K6" t="s">
         <v>89</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L6" t="s">
         <v>48</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M6" t="s">
         <v>43</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
         <v>157</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>133</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>129</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H7" t="s">
         <v>119</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" t="s">
         <v>111</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J7" t="s">
         <v>103</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K7" t="s">
         <v>90</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L7" t="s">
         <v>49</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
         <v>158</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>134</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>136</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>120</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J8" t="s">
         <v>104</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K8" t="s">
         <v>91</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L8" t="s">
         <v>50</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
         <v>159</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>135</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>144</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>121</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>113</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J9" t="s">
         <v>105</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K9" t="s">
         <v>92</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L9" t="s">
         <v>51</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
         <v>160</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>137</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>146</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>122</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I10" t="s">
         <v>114</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>106</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K10" t="s">
         <v>93</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L10" t="s">
         <v>52</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
         <v>161</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>138</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>123</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I11" t="s">
         <v>115</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>94</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L11" t="s">
         <v>53</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
         <v>162</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>141</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>140</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I12" t="s">
         <v>177</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>95</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>54</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M12" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H12" t="s">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
         <v>145</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K13" t="s">
         <v>96</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L13" t="s">
         <v>55</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M13" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K13" t="s">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="K14" t="s">
         <v>97</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L14" t="s">
         <v>56</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="K14" t="s">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="K15" t="s">
         <v>98</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L15" t="s">
         <v>57</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L15" t="s">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
         <v>58</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M16" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L16" t="s">
+    <row r="17" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
         <v>59</v>
       </c>
-      <c r="M16" t="s">
+      <c r="M17" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L17" t="s">
+    <row r="18" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
         <v>60</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L18" t="s">
+    <row r="19" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L19" t="s">
         <v>61</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M19" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L19" t="s">
+    <row r="20" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L20" t="s">
+    <row r="21" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L21" t="s">
+    <row r="22" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L22" t="s">
+    <row r="23" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L23" t="s">
+    <row r="24" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L24" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L24" t="s">
+    <row r="25" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L25" t="s">
+    <row r="26" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L26" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L26" t="s">
+    <row r="27" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L27" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L27" t="s">
+    <row r="28" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L28" t="s">
+    <row r="29" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L29" t="s">
+    <row r="30" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L30" t="s">
+    <row r="31" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L31" t="s">
+    <row r="32" spans="12:13" x14ac:dyDescent="0.3">
+      <c r="L32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L32" t="s">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L33" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L33" t="s">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L34" t="s">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L35" t="s">
+    <row r="36" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L36" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L36" t="s">
+    <row r="37" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L37" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L37" t="s">
+    <row r="38" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L38" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L38" t="s">
+    <row r="39" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L39" t="s">
+    <row r="40" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L40" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L40" t="s">
+    <row r="41" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L41" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L41" t="s">
+    <row r="42" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L42" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L42" t="s">
+    <row r="43" spans="12:12" x14ac:dyDescent="0.3">
+      <c r="L43" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G49">
-        <f ca="1">A43:G49</f>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G50">
+        <f ca="1">A44:G50</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ADD: Añadidos campos para comparar Sub.21 en paso5 sectorial
</commit_message>
<xml_diff>
--- a/applications/sectores_gubernamentales/Nomina Reparticiones Públicas.xlsx
+++ b/applications/sectores_gubernamentales/Nomina Reparticiones Públicas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaime\Desktop\SUBDERE\Transferencia de Competencias\transferenciacompetencias\applications\sectores_gubernamentales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1805CAF3-BFF4-4DC6-8418-4CF2106F3540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A65256-DAB7-44F8-8665-C5E6C93812F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -909,15 +909,15 @@
   <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="23" width="54.44140625" customWidth="1"/>
+    <col min="1" max="23" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -988,7 +988,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>152</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>151</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>157</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>158</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>159</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>160</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>161</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>162</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
         <v>145</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
         <v>97</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="K15" t="s">
         <v>98</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="L16" t="s">
         <v>58</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L17" t="s">
         <v>59</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L18" t="s">
         <v>60</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L19" t="s">
         <v>61</v>
       </c>
@@ -1486,127 +1486,127 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L24" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L26" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L27" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="12:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L33" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L36" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L37" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L38" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L40" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="41" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L41" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="42" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L42" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L43" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G50">
         <f ca="1">A44:G50</f>
         <v>0</v>

</xml_diff>

<commit_message>
FIX: Bugs para paso 3 sectorial y Nómina reparticiones públicas
</commit_message>
<xml_diff>
--- a/applications/sectores_gubernamentales/Nomina Reparticiones Públicas.xlsx
+++ b/applications/sectores_gubernamentales/Nomina Reparticiones Públicas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaime\Desktop\SUBDERE\Transferencia de Competencias\transferenciacompetencias\applications\sectores_gubernamentales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A65256-DAB7-44F8-8665-C5E6C93812F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EC6BDD-BEF3-41DD-88BE-D9DEA593DAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
   <si>
     <t>Ministerio del Interior y Seguridad Pública</t>
   </si>
@@ -570,9 +570,6 @@
   </si>
   <si>
     <t>Servicio Nacional de Reinserción Social Juvenil</t>
-  </si>
-  <si>
-    <t>Nivel Central</t>
   </si>
 </sst>
 </file>
@@ -906,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W50"/>
+  <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="W2" sqref="A2:W43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,74 +986,97 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G2" t="s">
-        <v>178</v>
-      </c>
-      <c r="H2" t="s">
-        <v>178</v>
-      </c>
-      <c r="I2" t="s">
-        <v>178</v>
-      </c>
-      <c r="J2" t="s">
-        <v>178</v>
-      </c>
-      <c r="K2" t="s">
-        <v>178</v>
-      </c>
-      <c r="L2" t="s">
-        <v>178</v>
-      </c>
-      <c r="M2" t="s">
-        <v>178</v>
-      </c>
-      <c r="N2" t="s">
-        <v>178</v>
-      </c>
-      <c r="O2" t="s">
-        <v>178</v>
-      </c>
-      <c r="P2" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>178</v>
-      </c>
-      <c r="R2" t="s">
-        <v>178</v>
-      </c>
-      <c r="S2" t="s">
-        <v>178</v>
-      </c>
-      <c r="T2" t="s">
-        <v>178</v>
-      </c>
-      <c r="U2" t="s">
-        <v>178</v>
-      </c>
-      <c r="V2" t="s">
-        <v>178</v>
-      </c>
-      <c r="W2" t="s">
-        <v>178</v>
+      <c r="A2" t="str">
+        <f t="shared" ref="A2:C2" si="0">_xlfn.CONCAT("Nivel Central - ",A1)</f>
+        <v>Nivel Central - Ministerio del Interior y Seguridad Pública</v>
+      </c>
+      <c r="B2" t="str">
+        <f t="shared" si="0"/>
+        <v>Nivel Central - Ministerio de Relaciones Exteriores</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" si="0"/>
+        <v>Nivel Central - Ministerio de Hacienda</v>
+      </c>
+      <c r="D2" t="str">
+        <f>_xlfn.CONCAT("Nivel Central - ",D1)</f>
+        <v>Nivel Central - Ministerio Secretaría General de la Presidencia</v>
+      </c>
+      <c r="E2" t="str">
+        <f>_xlfn.CONCAT("Nivel Central - ",E1)</f>
+        <v>Nivel Central - Ministerio Secretaría General de Gobierno</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:W2" si="1">_xlfn.CONCAT("Nivel Central - ",F1)</f>
+        <v>Nivel Central - Ministerio de Economía, Fomento y Turismo</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Desarrollo Social y Familia</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Educación</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Justicia y Derechos Humanos</v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio del Trabajo y Previsión Social</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Obras Públicas</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Salud</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Vivienda y Urbanismo</v>
+      </c>
+      <c r="N2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Agricultura</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Minería</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Transportes y Telecomunicaciones</v>
+      </c>
+      <c r="Q2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Bienes Nacionales</v>
+      </c>
+      <c r="R2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Energía</v>
+      </c>
+      <c r="S2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio del Medio Ambiente</v>
+      </c>
+      <c r="T2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio del Deporte</v>
+      </c>
+      <c r="U2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de la Mujer y la Equidad de Género</v>
+      </c>
+      <c r="V2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de las Culturas, las Artes y el Patrimonio</v>
+      </c>
+      <c r="W2" t="str">
+        <f t="shared" si="1"/>
+        <v>Nivel Central - Ministerio de Ciencia, Tecnología, Conocimiento e Innovación</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -1604,12 +1624,6 @@
     <row r="43" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L43" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G50">
-        <f ca="1">A44:G50</f>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>